<commit_message>
Update projections for external use, add ICWMT files
</commit_message>
<xml_diff>
--- a/Housing Archetypes/MatGHGint.xlsx
+++ b/Housing Archetypes/MatGHGint.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pb637\Documents\Yale Courses\Research\US Housing\Athena MI Archetypes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\Documents\projects\Yale\HSM_github\Housing Archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3DDCABD-719E-4F10-BE22-E91A7F1776DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B361895-A3E7-4A34-AA93-F6CCB089F34E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="105" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -1300,13 +1300,13 @@
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.3984375" customWidth="1"/>
-    <col min="2" max="3" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="2" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="str">
         <f>MetaData!A2</f>
         <v>Asphalt-saturated Felt</v>
@@ -1331,7 +1331,7 @@
         <v>0.31356783919597997</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="str">
         <f>MetaData!A3</f>
         <v>Gypsum Board</v>
@@ -1345,7 +1345,7 @@
         <v>0.23788371410219283</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="str">
         <f>MetaData!A4</f>
         <v>General Polyethylene</v>
@@ -1359,7 +1359,7 @@
         <v>2.23672</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="str">
         <f>MetaData!A5</f>
         <v>Aluminium</v>
@@ -1373,7 +1373,7 @@
         <v>2.8250000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="str">
         <f>MetaData!A6</f>
         <v>Cement</v>
@@ -1387,7 +1387,7 @@
         <v>0.7752</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="str">
         <f>MetaData!A7</f>
         <v>Concrete</v>
@@ -1401,7 +1401,7 @@
         <v>9.6799999999999997E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="str">
         <f>MetaData!A8</f>
         <v>Glass</v>
@@ -1415,7 +1415,7 @@
         <v>1.4669999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="str">
         <f>MetaData!A9</f>
         <v>Expanded Polystyrene</v>
@@ -1429,7 +1429,7 @@
         <v>3.8015400000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="str">
         <f>MetaData!A10</f>
         <v>Extruded Polystyrene</v>
@@ -1443,7 +1443,7 @@
         <v>12.605499999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="str">
         <f>MetaData!A11</f>
         <v>Fiberglass Insulation</v>
@@ -1457,7 +1457,7 @@
         <v>1.4899425287356323</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="str">
         <f>MetaData!A12</f>
         <v>Glass fibre reinforced plastic</v>
@@ -1471,7 +1471,7 @@
         <v>7.0684800000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="str">
         <f>MetaData!A13</f>
         <v>Steel</v>
@@ -1485,7 +1485,7 @@
         <v>1.4924999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="str">
         <f>MetaData!A14</f>
         <v>Fibrelass Shingles</v>
@@ -1499,7 +1499,7 @@
         <v>0.25736019782902758</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="str">
         <f>MetaData!A15</f>
         <v>Gypsum Joint Compound</v>
@@ -1513,7 +1513,7 @@
         <v>0.27869638826185106</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="str">
         <f>MetaData!A16</f>
         <v>Laminated Veneer Lumber</v>
@@ -1527,7 +1527,7 @@
         <v>0.24028210294925814</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="str">
         <f>MetaData!A17</f>
         <v>Lime</v>
@@ -1541,7 +1541,7 @@
         <v>0.70200000000000007</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="str">
         <f>MetaData!A18</f>
         <v>Oriented Strand Board</v>
@@ -1555,7 +1555,7 @@
         <v>0.25464657620700543</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="str">
         <f>MetaData!A19</f>
         <v>Timber</v>
@@ -1569,7 +1569,7 @@
         <v>8.9191304347826086E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="str">
         <f>MetaData!A20</f>
         <v>Paper</v>
@@ -1583,7 +1583,7 @@
         <v>0.83850000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="str">
         <f>MetaData!A21</f>
         <v>Plywood</v>
@@ -1597,7 +1597,7 @@
         <v>0.17172333061889253</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="str">
         <f>MetaData!A22</f>
         <v>Paint, solvent-based</v>
@@ -1611,7 +1611,7 @@
         <v>1.6644807494769602</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="str">
         <f>MetaData!A23</f>
         <v>Paint, water-based</v>
@@ -1625,7 +1625,7 @@
         <v>2.1698793779274594</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="str">
         <f>MetaData!A24</f>
         <v>Poly-iso insulation foam board</v>
@@ -1639,7 +1639,7 @@
         <v>3.2236249999999997</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="str">
         <f>MetaData!A25</f>
         <v>PVC</v>
@@ -1653,7 +1653,7 @@
         <v>1.5280800000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="str">
         <f>MetaData!A26</f>
         <v>Sand/Aggregate</v>
@@ -1667,7 +1667,7 @@
         <v>6.7229999999999998E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
         <f>MetaData!A27</f>
         <v>Brick</v>
@@ -1681,7 +1681,7 @@
         <v>0.189</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="str">
         <f>MetaData!A28</f>
         <v>TPO</v>
@@ -1695,7 +1695,7 @@
         <v>2.5723076923076924</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="str">
         <f>MetaData!A29</f>
         <v>EPDM</v>
@@ -1709,7 +1709,7 @@
         <v>2.5515789473684212</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="str">
         <f>MetaData!A30</f>
         <v xml:space="preserve">Asphalt  </v>
@@ -1723,7 +1723,7 @@
         <v>0.2646</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="str">
         <f>MetaData!A31</f>
         <v>Void</v>
@@ -1747,25 +1747,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66C82B7C-1C22-48CA-B5C1-79AFF004EF02}">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.6640625" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.06640625" customWidth="1"/>
-    <col min="4" max="4" width="42.19921875" customWidth="1"/>
-    <col min="5" max="5" width="92.19921875" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" customWidth="1"/>
+    <col min="4" max="4" width="42.21875" customWidth="1"/>
+    <col min="5" max="5" width="92.21875" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.46484375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.3984375" customWidth="1"/>
-    <col min="12" max="12" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" customWidth="1"/>
+    <col min="12" max="12" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>0.21299999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1905,7 +1905,7 @@
         <v>2.54</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>5.2673267326732676</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1961,7 +1961,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>0.12388002126592411</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2051,7 +2051,7 @@
         <v>2.7951993805652342</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>2.394179894179894</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>2.5291000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>0.47902827323694125</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>1.102803738317757E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>0.45500000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>0.26300000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>0.77809523809523806</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>0.68100000000000005</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>3.76</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>2.54</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>1.33587786259542</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>3.7820748059280174</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>64</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>2.222691356535376E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>0.15147392290249434</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>59</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>1.1384560111375579</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -2720,7 +2720,7 @@
         <v>0.33239038189533238</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>61</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>5.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -2784,31 +2784,31 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>115</v>
       </c>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H40" s="1"/>
     </row>
   </sheetData>

</xml_diff>